<commit_message>
actualización hasta week 6
actualización hasta week 6
</commit_message>
<xml_diff>
--- a/NoteBook/task and schedule plans and actual/TASK_Rafael_Ortega.xlsx
+++ b/NoteBook/task and schedule plans and actual/TASK_Rafael_Ortega.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Documents\GitHub\tsp\documentos\ciclo1\Rafael Ortega\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24526"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="14360" yWindow="0" windowWidth="14360" windowHeight="17560"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
   <si>
     <t>TSPi Example Task Planning Template - Form TASK</t>
   </si>
@@ -275,7 +273,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -283,58 +281,58 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -342,51 +340,51 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -437,11 +435,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -449,7 +447,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -461,15 +465,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -479,11 +474,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -545,7 +543,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -580,7 +578,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -757,7 +755,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -767,23 +765,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="4.85546875" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" customWidth="1"/>
+    <col min="3" max="3" width="38.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:13" ht="18">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -794,7 +792,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="2"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -809,7 +807,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="16.5" customHeight="1" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -821,7 +819,7 @@
       <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="31">
+      <c r="F3" s="17">
         <v>41718</v>
       </c>
       <c r="G3" s="18"/>
@@ -829,7 +827,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="16" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -849,7 +847,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="16" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -869,7 +867,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="15" thickBot="1">
       <c r="A6" s="2"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -884,147 +882,147 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
+    <row r="7" spans="1:13" ht="16" thickBot="1">
+      <c r="A7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="24" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="24" t="s">
+      <c r="E7" s="22"/>
+      <c r="F7" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="24" t="s">
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="25"/>
-      <c r="M7" s="26"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="22"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+    <row r="8" spans="1:13">
+      <c r="A8" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="K8" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="L8" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="M8" s="23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
+    <row r="9" spans="1:13">
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
+    <row r="10" spans="1:13">
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
+    <row r="11" spans="1:13">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
+    <row r="12" spans="1:13">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
     </row>
-    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
+    <row r="13" spans="1:13" ht="15" thickBot="1">
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
     </row>
-    <row r="14" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A14" s="29" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="4"/>
@@ -1066,8 +1064,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
+    <row r="15" spans="1:13" ht="15" customHeight="1" thickBot="1">
+      <c r="A15" s="30"/>
       <c r="B15" s="9"/>
       <c r="C15" s="5" t="s">
         <v>27</v>
@@ -1107,8 +1105,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
+    <row r="16" spans="1:13" ht="15" thickBot="1">
+      <c r="A16" s="31"/>
       <c r="B16" s="9"/>
       <c r="C16" s="5" t="s">
         <v>28</v>
@@ -1141,15 +1139,15 @@
         <v>0.4</v>
       </c>
       <c r="L16" s="8">
-        <f t="shared" ref="L16:L18" si="1">K16+L15</f>
+        <f t="shared" ref="L16:L36" si="1">K16+L15</f>
         <v>3.3</v>
       </c>
       <c r="M16" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16384" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
+    <row r="17" spans="1:16384" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A17" s="29" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="9"/>
@@ -1191,8 +1189,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
+    <row r="18" spans="1:16384" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A18" s="30"/>
       <c r="B18" s="9"/>
       <c r="C18" s="5" t="s">
         <v>31</v>
@@ -1232,8 +1230,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:16384" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
+    <row r="19" spans="1:16384" ht="16.5" customHeight="1" thickBot="1">
+      <c r="A19" s="29" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="9"/>
@@ -1268,14 +1266,15 @@
         <v>0.5</v>
       </c>
       <c r="L19" s="8">
+        <f t="shared" si="1"/>
         <v>6.3</v>
       </c>
       <c r="M19" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:16384" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
+    <row r="20" spans="1:16384" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A20" s="30"/>
       <c r="B20" s="9"/>
       <c r="C20" s="5" t="s">
         <v>34</v>
@@ -1308,14 +1307,15 @@
         <v>0.2</v>
       </c>
       <c r="L20" s="8">
+        <f t="shared" si="1"/>
         <v>6.5</v>
       </c>
       <c r="M20" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:16384" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
+    <row r="21" spans="1:16384" ht="15" customHeight="1" thickBot="1">
+      <c r="A21" s="30"/>
       <c r="B21" s="9"/>
       <c r="C21" s="5" t="s">
         <v>35</v>
@@ -1348,14 +1348,15 @@
         <v>0.6</v>
       </c>
       <c r="L21" s="8">
+        <f t="shared" si="1"/>
         <v>7.1</v>
       </c>
       <c r="M21" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:16384" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
+    <row r="22" spans="1:16384" ht="15" customHeight="1" thickBot="1">
+      <c r="A22" s="30"/>
       <c r="B22" s="9"/>
       <c r="C22" s="5" t="s">
         <v>36</v>
@@ -1388,14 +1389,15 @@
         <v>0.5</v>
       </c>
       <c r="L22" s="8">
+        <f t="shared" si="1"/>
         <v>7.6</v>
       </c>
       <c r="M22" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:16384" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
+    <row r="23" spans="1:16384" ht="15" customHeight="1" thickBot="1">
+      <c r="A23" s="30"/>
       <c r="B23" s="9"/>
       <c r="C23" s="5" t="s">
         <v>37</v>
@@ -1428,14 +1430,15 @@
         <v>1.9</v>
       </c>
       <c r="L23" s="8">
+        <f t="shared" si="1"/>
         <v>9.5</v>
       </c>
       <c r="M23" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:16384" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
+    <row r="24" spans="1:16384" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A24" s="31"/>
       <c r="B24" s="9"/>
       <c r="C24" s="5" t="s">
         <v>38</v>
@@ -1468,14 +1471,15 @@
         <v>3</v>
       </c>
       <c r="L24" s="8">
+        <f t="shared" si="1"/>
         <v>12.5</v>
       </c>
       <c r="M24" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:16384" s="14" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
+    <row r="25" spans="1:16384" s="14" customFormat="1" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A25" s="29" t="s">
         <v>39</v>
       </c>
       <c r="B25" s="12"/>
@@ -1506,9 +1510,16 @@
         <f t="shared" si="2"/>
         <v>45.2</v>
       </c>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
+      <c r="K25" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="L25" s="8">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="M25" s="8">
+        <v>4</v>
+      </c>
       <c r="N25" s="13"/>
       <c r="O25" s="13"/>
       <c r="P25" s="13"/>
@@ -17881,8 +17892,8 @@
       <c r="XFC25" s="13"/>
       <c r="XFD25" s="13"/>
     </row>
-    <row r="26" spans="1:16384" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
+    <row r="26" spans="1:16384" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A26" s="31"/>
       <c r="B26" s="12"/>
       <c r="C26" s="5" t="s">
         <v>54</v>
@@ -17911,12 +17922,19 @@
         <f t="shared" si="2"/>
         <v>48.5</v>
       </c>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
+      <c r="K26" s="8">
+        <v>3</v>
+      </c>
+      <c r="L26" s="8">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="M26" s="8">
+        <v>4</v>
+      </c>
     </row>
-    <row r="27" spans="1:16384" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
+    <row r="27" spans="1:16384" ht="15" customHeight="1" thickBot="1">
+      <c r="A27" s="29" t="s">
         <v>41</v>
       </c>
       <c r="B27" s="15"/>
@@ -17930,7 +17948,9 @@
         <f t="shared" si="0"/>
         <v>15.5</v>
       </c>
-      <c r="F27" s="6"/>
+      <c r="F27" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="G27" s="8">
         <v>3</v>
       </c>
@@ -17945,12 +17965,19 @@
         <f t="shared" si="2"/>
         <v>51.8</v>
       </c>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
+      <c r="K27" s="8">
+        <v>1.8</v>
+      </c>
+      <c r="L27" s="8">
+        <f t="shared" si="1"/>
+        <v>19.8</v>
+      </c>
+      <c r="M27" s="8">
+        <v>4</v>
+      </c>
     </row>
-    <row r="28" spans="1:16384" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="20"/>
+    <row r="28" spans="1:16384" ht="17.25" customHeight="1" thickBot="1">
+      <c r="A28" s="30"/>
       <c r="B28" s="9"/>
       <c r="C28" s="5" t="s">
         <v>42</v>
@@ -17979,12 +18006,19 @@
         <f t="shared" si="2"/>
         <v>55.099999999999994</v>
       </c>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
+      <c r="K28" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="L28" s="8">
+        <f t="shared" si="1"/>
+        <v>20.7</v>
+      </c>
+      <c r="M28" s="8">
+        <v>4</v>
+      </c>
     </row>
-    <row r="29" spans="1:16384" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="20"/>
+    <row r="29" spans="1:16384" ht="16.5" customHeight="1" thickBot="1">
+      <c r="A29" s="30"/>
       <c r="B29" s="9"/>
       <c r="C29" s="5" t="s">
         <v>56</v>
@@ -18013,12 +18047,19 @@
         <f t="shared" si="2"/>
         <v>61.8</v>
       </c>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
+      <c r="K29" s="8">
+        <v>2.1</v>
+      </c>
+      <c r="L29" s="8">
+        <f t="shared" si="1"/>
+        <v>22.8</v>
+      </c>
+      <c r="M29" s="8">
+        <v>4</v>
+      </c>
     </row>
-    <row r="30" spans="1:16384" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="17"/>
+    <row r="30" spans="1:16384" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A30" s="31"/>
       <c r="B30" s="9"/>
       <c r="C30" s="5" t="s">
         <v>43</v>
@@ -18047,12 +18088,19 @@
         <f t="shared" si="2"/>
         <v>65.099999999999994</v>
       </c>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
+      <c r="K30" s="8">
+        <v>1.3</v>
+      </c>
+      <c r="L30" s="8">
+        <f t="shared" si="1"/>
+        <v>24.1</v>
+      </c>
+      <c r="M30" s="8">
+        <v>4</v>
+      </c>
     </row>
-    <row r="31" spans="1:16384" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="16" t="s">
+    <row r="31" spans="1:16384" ht="17.25" customHeight="1" thickBot="1">
+      <c r="A31" s="29" t="s">
         <v>44</v>
       </c>
       <c r="B31" s="9"/>
@@ -18083,12 +18131,19 @@
         <f t="shared" si="2"/>
         <v>68.399999999999991</v>
       </c>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
+      <c r="K31" s="8">
+        <v>1.8</v>
+      </c>
+      <c r="L31" s="8">
+        <f t="shared" si="1"/>
+        <v>25.900000000000002</v>
+      </c>
+      <c r="M31" s="8">
+        <v>5</v>
+      </c>
     </row>
-    <row r="32" spans="1:16384" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="20"/>
+    <row r="32" spans="1:16384" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A32" s="30"/>
       <c r="B32" s="9"/>
       <c r="C32" s="5" t="s">
         <v>45</v>
@@ -18113,12 +18168,19 @@
         <f t="shared" si="2"/>
         <v>71.699999999999989</v>
       </c>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
+      <c r="K32" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="L32" s="8">
+        <f t="shared" si="1"/>
+        <v>26.6</v>
+      </c>
+      <c r="M32" s="8">
+        <v>5</v>
+      </c>
     </row>
-    <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="20"/>
+    <row r="33" spans="1:13" ht="15" thickBot="1">
+      <c r="A33" s="30"/>
       <c r="B33" s="9"/>
       <c r="C33" s="5" t="s">
         <v>46</v>
@@ -18147,11 +18209,18 @@
         <f t="shared" si="2"/>
         <v>88.399999999999991</v>
       </c>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
+      <c r="K33" s="8">
+        <v>6.2</v>
+      </c>
+      <c r="L33" s="8">
+        <f t="shared" si="1"/>
+        <v>32.800000000000004</v>
+      </c>
+      <c r="M33" s="8">
+        <v>5</v>
+      </c>
     </row>
-    <row r="34" spans="1:13" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" ht="17.25" customHeight="1" thickBot="1">
       <c r="A34" s="10" t="s">
         <v>48</v>
       </c>
@@ -18183,12 +18252,19 @@
         <f t="shared" si="2"/>
         <v>91.699999999999989</v>
       </c>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
+      <c r="K34" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="L34" s="8">
+        <f t="shared" si="1"/>
+        <v>33.500000000000007</v>
+      </c>
+      <c r="M34" s="8">
+        <v>5</v>
+      </c>
     </row>
-    <row r="35" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="16" t="s">
+    <row r="35" spans="1:13" ht="15" customHeight="1" thickBot="1">
+      <c r="A35" s="29" t="s">
         <v>50</v>
       </c>
       <c r="B35" s="9"/>
@@ -18219,12 +18295,19 @@
         <f t="shared" si="2"/>
         <v>94.999999999999986</v>
       </c>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
+      <c r="K35" s="8">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L35" s="8">
+        <f t="shared" si="1"/>
+        <v>35.800000000000004</v>
+      </c>
+      <c r="M35" s="8">
+        <v>6</v>
+      </c>
     </row>
-    <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="17"/>
+    <row r="36" spans="1:13" ht="15" thickBot="1">
+      <c r="A36" s="31"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12" t="s">
         <v>52</v>
@@ -18253,11 +18336,18 @@
         <f t="shared" si="2"/>
         <v>99.999999999999986</v>
       </c>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
+      <c r="K36" s="8">
+        <v>1.8</v>
+      </c>
+      <c r="L36" s="8">
+        <f t="shared" si="1"/>
+        <v>37.6</v>
+      </c>
+      <c r="M36" s="8">
+        <v>6</v>
+      </c>
     </row>
-    <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" ht="15" thickBot="1">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -18277,11 +18367,19 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="G8:G13"/>
     <mergeCell ref="K7:M7"/>
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="B8:B13"/>
@@ -18290,25 +18388,22 @@
     <mergeCell ref="E8:E13"/>
     <mergeCell ref="F8:F13"/>
     <mergeCell ref="M8:M13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="G8:G13"/>
     <mergeCell ref="H8:H13"/>
     <mergeCell ref="I8:I13"/>
     <mergeCell ref="J8:J13"/>
     <mergeCell ref="K8:K13"/>
     <mergeCell ref="L8:L13"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F7:J7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>